<commit_message>
tính năng tải lên khsx 90%
</commit_message>
<xml_diff>
--- a/vdm_lk2_machine/database/FORM KẾ HOẠCH SẢN XUẤT CÔNG ĐOẠN THÀNH HÌNH.xlsx
+++ b/vdm_lk2_machine/database/FORM KẾ HOẠCH SẢN XUẤT CÔNG ĐOẠN THÀNH HÌNH.xlsx
@@ -565,10 +565,10 @@
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="10.71"/>
@@ -674,7 +674,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="6" t="n">
-        <v>38160</v>
+        <v>40000</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>38160</v>

</xml_diff>